<commit_message>
29 May Data updates
</commit_message>
<xml_diff>
--- a/data/Key Metrics.xlsx
+++ b/data/Key Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD5EBD9-7B66-46B5-8369-CD1932BC4A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B165ED-3F8E-44C9-9FF7-2120A2E92BA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11100" xr2:uid="{A53410EC-0570-4A6D-8CC6-C38FD68A563E}"/>
   </bookViews>
@@ -426,13 +426,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2973B47C-AFF3-40C0-9DB8-6623AA76EC61}">
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J131" sqref="J131"/>
+      <selection pane="bottomRight" activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,19 +1613,19 @@
         <v>60</v>
       </c>
       <c r="C53">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="0"/>
-        <v>6.3761955366631248E-2</v>
+        <v>6.3897763578274758E-2</v>
       </c>
       <c r="F53">
         <f t="shared" si="2"/>
-        <v>0.10438074634937804</v>
+        <v>0.1044937736870601</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="0"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="F54">
         <f t="shared" si="2"/>
-        <v>8.3208395802098947E-2</v>
+        <v>8.3270817704426112E-2</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -1659,19 +1659,19 @@
         <v>68</v>
       </c>
       <c r="C55">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D55">
         <f>C55+D54</f>
-        <v>3910</v>
+        <v>3907</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" si="0"/>
-        <v>6.5700483091787443E-2</v>
+        <v>6.5764023210831718E-2</v>
       </c>
       <c r="F55">
         <f t="shared" ref="F55:F60" si="3">IFERROR(SUMPRODUCT(C49:C55,E49:E55)/SUM(C49:C55),"")</f>
-        <v>7.4266922444505348E-2</v>
+        <v>7.4328030718595728E-2</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -1682,19 +1682,19 @@
         <v>150</v>
       </c>
       <c r="C56">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="D56">
         <f t="shared" si="1"/>
-        <v>6062</v>
+        <v>6057</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="0"/>
-        <v>6.9702602230483274E-2</v>
+        <v>6.9767441860465115E-2</v>
       </c>
       <c r="F56">
         <f t="shared" si="3"/>
-        <v>7.2625698324022353E-2</v>
+        <v>7.2689149047702253E-2</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -1705,19 +1705,19 @@
         <v>249</v>
       </c>
       <c r="C57">
-        <v>2686</v>
+        <v>2685</v>
       </c>
       <c r="D57">
         <f t="shared" si="1"/>
-        <v>8748</v>
+        <v>8742</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="0"/>
-        <v>9.2702903946388679E-2</v>
+        <v>9.2737430167597765E-2</v>
       </c>
       <c r="F57">
         <f t="shared" si="3"/>
-        <v>7.834877843302443E-2</v>
+        <v>7.8405395640130077E-2</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -1728,19 +1728,19 @@
         <v>259</v>
       </c>
       <c r="C58">
-        <v>2993</v>
+        <v>2994</v>
       </c>
       <c r="D58">
         <f t="shared" si="1"/>
-        <v>11741</v>
+        <v>11736</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="0"/>
-        <v>8.6535248914132973E-2</v>
+        <v>8.6506346025384095E-2</v>
       </c>
       <c r="F58">
         <f t="shared" si="3"/>
-        <v>7.979870596693027E-2</v>
+        <v>7.983457700260721E-2</v>
       </c>
       <c r="J58">
         <v>2</v>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="D59">
         <f t="shared" si="1"/>
-        <v>14646</v>
+        <v>14641</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="0"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="F59">
         <f t="shared" si="3"/>
-        <v>8.3510833639368343E-2</v>
+        <v>8.3541513592946356E-2</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -1777,22 +1777,22 @@
         <v>43910</v>
       </c>
       <c r="B60">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C60">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="D60">
         <f t="shared" si="1"/>
-        <v>18297</v>
+        <v>18291</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="0"/>
-        <v>0.10627225417693782</v>
+        <v>0.10602739726027398</v>
       </c>
       <c r="F60">
         <f t="shared" si="3"/>
-        <v>8.9739663093415009E-2</v>
+        <v>8.9700386005759455E-2</v>
       </c>
       <c r="J60">
         <v>2</v>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D61">
         <f t="shared" si="1"/>
-        <v>20832</v>
+        <v>20826</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="0"/>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="F61">
         <f t="shared" si="2"/>
-        <v>9.5338865066547859E-2</v>
+        <v>9.530440594886648E-2</v>
       </c>
       <c r="J61">
         <v>2</v>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="D62">
         <f t="shared" si="1"/>
-        <v>22730</v>
+        <v>22724</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="0"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="F62">
         <f t="shared" si="2"/>
-        <v>0.10255047821466524</v>
+        <v>0.10251368443428814</v>
       </c>
       <c r="J62">
         <v>4</v>
@@ -1870,19 +1870,19 @@
         <v>608</v>
       </c>
       <c r="C63">
-        <v>3797</v>
+        <v>3795</v>
       </c>
       <c r="D63">
         <f t="shared" si="1"/>
-        <v>26527</v>
+        <v>26519</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="0"/>
-        <v>0.16012641559125626</v>
+        <v>0.16021080368906457</v>
       </c>
       <c r="F63">
         <f t="shared" si="2"/>
-        <v>0.11668702663083313</v>
+        <v>0.11665526341511094</v>
       </c>
       <c r="J63">
         <v>6</v>
@@ -1900,19 +1900,19 @@
         <v>717</v>
       </c>
       <c r="C64">
-        <v>4007</v>
+        <v>4003</v>
       </c>
       <c r="D64">
         <f t="shared" si="1"/>
-        <v>30534</v>
+        <v>30522</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="0"/>
-        <v>0.17893686049413526</v>
+        <v>0.17911566325256059</v>
       </c>
       <c r="F64">
         <f t="shared" si="2"/>
-        <v>0.13109336270999725</v>
+        <v>0.13108356290174472</v>
       </c>
       <c r="J64">
         <v>9</v>
@@ -1927,22 +1927,22 @@
         <v>43915</v>
       </c>
       <c r="B65">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C65">
-        <v>4111</v>
+        <v>4108</v>
       </c>
       <c r="D65">
         <f t="shared" si="1"/>
-        <v>34645</v>
+        <v>34630</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="0"/>
-        <v>0.18097786426660181</v>
+        <v>0.18086660175267771</v>
       </c>
       <c r="F65">
         <f t="shared" si="2"/>
-        <v>0.14586971707998603</v>
+        <v>0.14584607320695378</v>
       </c>
       <c r="J65">
         <v>7</v>
@@ -1957,22 +1957,22 @@
         <v>43916</v>
       </c>
       <c r="B66">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C66">
-        <v>4432</v>
+        <v>4428</v>
       </c>
       <c r="D66">
         <f t="shared" si="1"/>
-        <v>39077</v>
+        <v>39058</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" si="0"/>
-        <v>0.21096570397111913</v>
+        <v>0.2109304426377597</v>
       </c>
       <c r="F66">
         <f t="shared" si="2"/>
-        <v>0.16364454995702182</v>
+        <v>0.16361551378138181</v>
       </c>
       <c r="J66">
         <v>9</v>
@@ -1990,19 +1990,19 @@
         <v>944</v>
       </c>
       <c r="C67">
-        <v>4384</v>
+        <v>4381</v>
       </c>
       <c r="D67">
         <f t="shared" si="1"/>
-        <v>43461</v>
+        <v>43439</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" ref="E67:E118" si="5">B67/C67</f>
-        <v>0.21532846715328466</v>
+        <v>0.21547591874001371</v>
       </c>
       <c r="F67">
         <f t="shared" si="2"/>
-        <v>0.18097281831187412</v>
+        <v>0.18100843009384443</v>
       </c>
       <c r="J67">
         <v>15</v>
@@ -2020,19 +2020,19 @@
         <v>655</v>
       </c>
       <c r="C68">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="D68">
         <f t="shared" ref="D68:D117" si="6">C68+D67</f>
-        <v>46271</v>
+        <v>46248</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="5"/>
-        <v>0.23309608540925267</v>
+        <v>0.23317906728373086</v>
       </c>
       <c r="F68">
         <f t="shared" si="2"/>
-        <v>0.19218522740673769</v>
+        <v>0.19223507198489498</v>
       </c>
       <c r="J68">
         <v>15</v>
@@ -2047,22 +2047,22 @@
         <v>43919</v>
       </c>
       <c r="B69">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C69">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="D69">
         <f t="shared" si="6"/>
-        <v>48354</v>
+        <v>48330</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="5"/>
-        <v>0.25060009601536248</v>
+        <v>0.25120076849183476</v>
       </c>
       <c r="F69">
         <f t="shared" si="2"/>
-        <v>0.20000780518264127</v>
+        <v>0.20010934937124111</v>
       </c>
       <c r="J69">
         <v>25</v>
@@ -2077,22 +2077,22 @@
         <v>43920</v>
       </c>
       <c r="B70">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C70">
-        <v>5070</v>
+        <v>5067</v>
       </c>
       <c r="D70">
         <f t="shared" si="6"/>
-        <v>53424</v>
+        <v>53397</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="5"/>
-        <v>0.24378698224852072</v>
+        <v>0.24373396487073218</v>
       </c>
       <c r="F70">
         <f t="shared" si="2"/>
-        <v>0.21389002490984124</v>
+        <v>0.21396681300692016</v>
       </c>
       <c r="J70">
         <v>28</v>
@@ -2110,19 +2110,19 @@
         <v>1266</v>
       </c>
       <c r="C71">
-        <v>5256</v>
+        <v>5254</v>
       </c>
       <c r="D71">
         <f t="shared" si="6"/>
-        <v>58680</v>
+        <v>58651</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="5"/>
-        <v>0.2408675799086758</v>
+        <v>0.24095926912828322</v>
       </c>
       <c r="F71">
         <f t="shared" si="2"/>
-        <v>0.22390392951040999</v>
+        <v>0.22396814675246188</v>
       </c>
       <c r="J71">
         <v>28</v>
@@ -2137,22 +2137,22 @@
         <v>43922</v>
       </c>
       <c r="B72">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="C72">
-        <v>4943</v>
+        <v>4942</v>
       </c>
       <c r="D72">
         <f t="shared" si="6"/>
-        <v>63623</v>
+        <v>63593</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="5"/>
-        <v>0.27068581832895006</v>
+        <v>0.2709429380817483</v>
       </c>
       <c r="F72">
         <f t="shared" si="2"/>
-        <v>0.23797363517150943</v>
+        <v>0.23809688222905087</v>
       </c>
       <c r="J72">
         <v>36</v>
@@ -2170,19 +2170,19 @@
         <v>1280</v>
       </c>
       <c r="C73">
-        <v>5254</v>
+        <v>5248</v>
       </c>
       <c r="D73">
         <f t="shared" si="6"/>
-        <v>68877</v>
+        <v>68841</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="5"/>
-        <v>0.24362390559573657</v>
+        <v>0.24390243902439024</v>
       </c>
       <c r="F73">
         <f t="shared" ref="F73:F118" si="7">IFERROR(SUMPRODUCT(C67:C73,E67:E73)/SUM(C67:C73),"")</f>
-        <v>0.24298657718120806</v>
+        <v>0.24315884900782325</v>
       </c>
       <c r="J73">
         <v>42</v>
@@ -2200,19 +2200,19 @@
         <v>1482</v>
       </c>
       <c r="C74">
-        <v>5791</v>
+        <v>5787</v>
       </c>
       <c r="D74">
         <f t="shared" si="6"/>
-        <v>74668</v>
+        <v>74628</v>
       </c>
       <c r="E74" s="3">
         <f t="shared" si="5"/>
-        <v>0.25591434985322054</v>
+        <v>0.25609123898392949</v>
       </c>
       <c r="F74">
         <f t="shared" si="7"/>
-        <v>0.24927099689172302</v>
+        <v>0.24944692038859853</v>
       </c>
       <c r="G74">
         <v>639</v>
@@ -2233,22 +2233,22 @@
         <v>43925</v>
       </c>
       <c r="B75">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C75">
-        <v>4009</v>
+        <v>4006</v>
       </c>
       <c r="D75">
         <f t="shared" si="6"/>
-        <v>78677</v>
+        <v>78634</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="5"/>
-        <v>0.29009728111748567</v>
+        <v>0.29006490264603096</v>
       </c>
       <c r="F75">
         <f t="shared" si="7"/>
-        <v>0.25572424859593901</v>
+        <v>0.25588217130859015</v>
       </c>
       <c r="G75">
         <v>1370</v>
@@ -2272,19 +2272,19 @@
         <v>976</v>
       </c>
       <c r="C76">
-        <v>3446</v>
+        <v>3439</v>
       </c>
       <c r="D76">
         <f t="shared" si="6"/>
-        <v>82123</v>
+        <v>82073</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="5"/>
-        <v>0.2832269297736506</v>
+        <v>0.28380343123000873</v>
       </c>
       <c r="F76">
         <f t="shared" si="7"/>
-        <v>0.25884687139092066</v>
+        <v>0.25901668494206204</v>
       </c>
       <c r="G76">
         <v>1632</v>
@@ -2309,22 +2309,22 @@
         <v>43927</v>
       </c>
       <c r="B77">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="C77">
-        <v>6710</v>
+        <v>6704</v>
       </c>
       <c r="D77">
         <f t="shared" si="6"/>
-        <v>88833</v>
+        <v>88777</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="5"/>
-        <v>0.28807749627421758</v>
+        <v>0.28818615751789978</v>
       </c>
       <c r="F77">
         <f t="shared" si="7"/>
-        <v>0.26654240447343897</v>
+        <v>0.26673261729790843</v>
       </c>
       <c r="G77">
         <v>1677</v>
@@ -2349,22 +2349,22 @@
         <v>43928</v>
       </c>
       <c r="B78">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C78">
-        <v>6623</v>
+        <v>6617</v>
       </c>
       <c r="D78">
         <f t="shared" si="6"/>
-        <v>95456</v>
+        <v>95394</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="5"/>
-        <v>0.3063566359655745</v>
+        <v>0.30633217470152635</v>
       </c>
       <c r="F78">
         <f t="shared" si="7"/>
-        <v>0.27738198825320859</v>
+        <v>0.27754946520425661</v>
       </c>
       <c r="G78">
         <v>1831</v>
@@ -2392,19 +2392,19 @@
         <v>1868</v>
       </c>
       <c r="C79">
-        <v>6847</v>
+        <v>6843</v>
       </c>
       <c r="D79">
         <f t="shared" si="6"/>
-        <v>102303</v>
+        <v>102237</v>
       </c>
       <c r="E79" s="3">
         <f t="shared" si="5"/>
-        <v>0.27282021323207245</v>
+        <v>0.2729796872716645</v>
       </c>
       <c r="F79">
         <f t="shared" si="7"/>
-        <v>0.27743019648397105</v>
+        <v>0.27758513611427388</v>
       </c>
       <c r="G79">
         <v>2119</v>
@@ -2429,22 +2429,22 @@
         <v>43930</v>
       </c>
       <c r="B80">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="C80">
-        <v>6506</v>
+        <v>6499</v>
       </c>
       <c r="D80">
         <f t="shared" si="6"/>
-        <v>108809</v>
+        <v>108736</v>
       </c>
       <c r="E80" s="3">
         <f t="shared" si="5"/>
-        <v>0.30571779895481094</v>
+        <v>0.30620095399292196</v>
       </c>
       <c r="F80">
         <f t="shared" si="7"/>
-        <v>0.28648702794751074</v>
+        <v>0.2866775285123449</v>
       </c>
       <c r="G80">
         <v>2302</v>
@@ -2469,22 +2469,22 @@
         <v>43931</v>
       </c>
       <c r="B81">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="C81">
-        <v>7677</v>
+        <v>7671</v>
       </c>
       <c r="D81">
         <f t="shared" si="6"/>
-        <v>116486</v>
+        <v>116407</v>
       </c>
       <c r="E81" s="3">
         <f t="shared" si="5"/>
-        <v>0.26859450306109156</v>
+        <v>0.26854386651023332</v>
       </c>
       <c r="F81">
         <f t="shared" si="7"/>
-        <v>0.28743603233057535</v>
+        <v>0.28758467172502933</v>
       </c>
       <c r="G81">
         <v>2435</v>
@@ -2512,19 +2512,19 @@
         <v>1300</v>
       </c>
       <c r="C82">
-        <v>4399</v>
+        <v>4395</v>
       </c>
       <c r="D82">
         <f t="shared" si="6"/>
-        <v>120885</v>
+        <v>120802</v>
       </c>
       <c r="E82" s="3">
         <f t="shared" si="5"/>
-        <v>0.29552170947942713</v>
+        <v>0.29579067121729236</v>
       </c>
       <c r="F82">
         <f t="shared" si="7"/>
-        <v>0.28802596664139501</v>
+        <v>0.28820432555492315</v>
       </c>
       <c r="G82">
         <v>2507</v>
@@ -2552,19 +2552,19 @@
         <v>931</v>
       </c>
       <c r="C83">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="D83">
         <f t="shared" si="6"/>
-        <v>124000</v>
+        <v>123915</v>
       </c>
       <c r="E83" s="3">
         <f t="shared" si="5"/>
-        <v>0.29887640449438202</v>
+        <v>0.29906842274333439</v>
       </c>
       <c r="F83">
         <f t="shared" si="7"/>
-        <v>0.2892279771712396</v>
+        <v>0.28937431289135318</v>
       </c>
       <c r="G83">
         <v>2554</v>
@@ -2592,19 +2592,19 @@
         <v>2002</v>
       </c>
       <c r="C84">
-        <v>6376</v>
+        <v>6374</v>
       </c>
       <c r="D84">
         <f t="shared" si="6"/>
-        <v>130376</v>
+        <v>130289</v>
       </c>
       <c r="E84" s="3">
         <f t="shared" si="5"/>
-        <v>0.31398996235884569</v>
+        <v>0.31408848446815185</v>
       </c>
       <c r="F84">
         <f t="shared" si="7"/>
-        <v>0.29321425992345279</v>
+        <v>0.29336095586818267</v>
       </c>
       <c r="G84">
         <v>3485</v>
@@ -2632,19 +2632,19 @@
         <v>2876</v>
       </c>
       <c r="C85">
-        <v>9810</v>
+        <v>9806</v>
       </c>
       <c r="D85">
         <f t="shared" si="6"/>
-        <v>140186</v>
+        <v>140095</v>
       </c>
       <c r="E85" s="3">
         <f t="shared" si="5"/>
-        <v>0.29317023445463813</v>
+        <v>0.29328982255761776</v>
       </c>
       <c r="F85">
         <f t="shared" si="7"/>
-        <v>0.29125866308964898</v>
+        <v>0.29142524775732087</v>
       </c>
       <c r="G85">
         <v>3616</v>
@@ -2669,22 +2669,22 @@
         <v>43936</v>
       </c>
       <c r="B86">
-        <v>2601</v>
+        <v>2602</v>
       </c>
       <c r="C86">
-        <v>10046</v>
+        <v>10034</v>
       </c>
       <c r="D86">
         <f t="shared" si="6"/>
-        <v>150232</v>
+        <v>150129</v>
       </c>
       <c r="E86" s="3">
         <f t="shared" si="5"/>
-        <v>0.25890901851483178</v>
+        <v>0.25931831771975283</v>
       </c>
       <c r="F86">
         <f t="shared" si="7"/>
-        <v>0.28711218677627326</v>
+        <v>0.28733400150338262</v>
       </c>
       <c r="G86">
         <v>3637</v>
@@ -2712,19 +2712,19 @@
         <v>2388</v>
       </c>
       <c r="C87">
-        <v>9001</v>
+        <v>8987</v>
       </c>
       <c r="D87">
         <f t="shared" si="6"/>
-        <v>159233</v>
+        <v>159116</v>
       </c>
       <c r="E87" s="3">
         <f t="shared" si="5"/>
-        <v>0.26530385512720811</v>
+        <v>0.2657171469900968</v>
       </c>
       <c r="F87">
         <f t="shared" si="7"/>
-        <v>0.28081865778200854</v>
+        <v>0.28104406510520047</v>
       </c>
       <c r="G87">
         <v>3726</v>
@@ -2749,22 +2749,22 @@
         <v>43938</v>
       </c>
       <c r="B88">
-        <v>3008</v>
+        <v>3009</v>
       </c>
       <c r="C88">
-        <v>11237</v>
+        <v>11223</v>
       </c>
       <c r="D88">
         <f t="shared" si="6"/>
-        <v>170470</v>
+        <v>170339</v>
       </c>
       <c r="E88" s="3">
         <f t="shared" si="5"/>
-        <v>0.26768710509922578</v>
+        <v>0.2681101309810211</v>
       </c>
       <c r="F88">
         <f t="shared" si="7"/>
-        <v>0.27982365145228216</v>
+        <v>0.28013053474745975</v>
       </c>
       <c r="G88">
         <v>3756</v>
@@ -2792,19 +2792,19 @@
         <v>1486</v>
       </c>
       <c r="C89">
-        <v>6136</v>
+        <v>6125</v>
       </c>
       <c r="D89">
         <f t="shared" si="6"/>
-        <v>176606</v>
+        <v>176464</v>
       </c>
       <c r="E89" s="3">
         <f t="shared" si="5"/>
-        <v>0.24217731421121252</v>
+        <v>0.24261224489795918</v>
       </c>
       <c r="F89">
         <f t="shared" si="7"/>
-        <v>0.2744387214874105</v>
+        <v>0.27476554920771801</v>
       </c>
       <c r="G89">
         <v>3728</v>
@@ -2829,22 +2829,22 @@
         <v>43940</v>
       </c>
       <c r="B90">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C90">
-        <v>4631</v>
+        <v>4627</v>
       </c>
       <c r="D90">
         <f t="shared" si="6"/>
-        <v>181237</v>
+        <v>181091</v>
       </c>
       <c r="E90" s="3">
         <f t="shared" si="5"/>
-        <v>0.23580220254804579</v>
+        <v>0.23578992867948995</v>
       </c>
       <c r="F90">
         <f t="shared" si="7"/>
-        <v>0.26998270349599035</v>
+        <v>0.27028823282496151</v>
       </c>
       <c r="G90">
         <v>3789</v>
@@ -2857,11 +2857,11 @@
         <v>25</v>
       </c>
       <c r="J90">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K90">
         <f t="shared" si="4"/>
-        <v>170.66666666666666</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -2869,22 +2869,22 @@
         <v>43941</v>
       </c>
       <c r="B91">
-        <v>2699</v>
+        <v>2700</v>
       </c>
       <c r="C91">
-        <v>10924</v>
+        <v>10904</v>
       </c>
       <c r="D91">
         <f t="shared" si="6"/>
-        <v>192161</v>
+        <v>191995</v>
       </c>
       <c r="E91" s="3">
         <f t="shared" si="5"/>
-        <v>0.24707067008421824</v>
+        <v>0.24761555392516507</v>
       </c>
       <c r="F91">
         <f t="shared" si="7"/>
-        <v>0.26139030509023226</v>
+        <v>0.26175736557222962</v>
       </c>
       <c r="G91">
         <v>3867</v>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="K91">
         <f t="shared" si="4"/>
-        <v>171.33333333333334</v>
+        <v>171.66666666666666</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -2909,22 +2909,22 @@
         <v>43942</v>
       </c>
       <c r="B92">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="C92">
-        <v>9570</v>
+        <v>9561</v>
       </c>
       <c r="D92">
         <f t="shared" si="6"/>
-        <v>201731</v>
+        <v>201556</v>
       </c>
       <c r="E92" s="3">
         <f t="shared" si="5"/>
-        <v>0.23009404388714733</v>
+        <v>0.23010145382282188</v>
       </c>
       <c r="F92">
         <f t="shared" si="7"/>
-        <v>0.25145828255747826</v>
+        <v>0.25180195571175218</v>
       </c>
       <c r="G92">
         <v>3965</v>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="K92">
         <f t="shared" si="4"/>
-        <v>169.33333333333334</v>
+        <v>169.66666666666666</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -2949,22 +2949,22 @@
         <v>43943</v>
       </c>
       <c r="B93">
-        <v>2722</v>
+        <v>2719</v>
       </c>
       <c r="C93">
-        <v>12701</v>
+        <v>12680</v>
       </c>
       <c r="D93">
         <f t="shared" si="6"/>
-        <v>214432</v>
+        <v>214236</v>
       </c>
       <c r="E93" s="3">
         <f t="shared" si="5"/>
-        <v>0.21431383355641287</v>
+        <v>0.21443217665615141</v>
       </c>
       <c r="F93">
         <f t="shared" si="7"/>
-        <v>0.24294392523364486</v>
+        <v>0.24323396820939991</v>
       </c>
       <c r="G93">
         <v>3873</v>
@@ -2989,22 +2989,22 @@
         <v>43944</v>
       </c>
       <c r="B94">
-        <v>2419</v>
+        <v>2420</v>
       </c>
       <c r="C94">
-        <v>10806</v>
+        <v>10790</v>
       </c>
       <c r="D94">
         <f t="shared" si="6"/>
-        <v>225238</v>
+        <v>225026</v>
       </c>
       <c r="E94" s="3">
         <f t="shared" si="5"/>
-        <v>0.22385711641680547</v>
+        <v>0.2242817423540315</v>
       </c>
       <c r="F94">
         <f t="shared" si="7"/>
-        <v>0.23676994167108553</v>
+        <v>0.23706569564557731</v>
       </c>
       <c r="G94">
         <v>3830</v>
@@ -3017,11 +3017,11 @@
         <v>21</v>
       </c>
       <c r="J94">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K94">
         <f t="shared" si="4"/>
-        <v>167.33333333333334</v>
+        <v>167.66666666666666</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -3032,19 +3032,19 @@
         <v>2277</v>
       </c>
       <c r="C95">
-        <v>12338</v>
+        <v>12321</v>
       </c>
       <c r="D95">
         <f t="shared" si="6"/>
-        <v>237576</v>
+        <v>237347</v>
       </c>
       <c r="E95" s="3">
         <f t="shared" si="5"/>
-        <v>0.1845517912141352</v>
+        <v>0.18480642804967129</v>
       </c>
       <c r="F95">
         <f t="shared" si="7"/>
-        <v>0.22199207224391262</v>
+        <v>0.22225704393505252</v>
       </c>
       <c r="G95">
         <v>3830</v>
@@ -3057,11 +3057,11 @@
         <v>22</v>
       </c>
       <c r="J95">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K95">
         <f t="shared" si="4"/>
-        <v>178.66666666666666</v>
+        <v>179.33333333333334</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -3069,22 +3069,22 @@
         <v>43946</v>
       </c>
       <c r="B96">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="C96">
-        <v>8366</v>
+        <v>8351</v>
       </c>
       <c r="D96">
         <f t="shared" si="6"/>
-        <v>245942</v>
+        <v>245698</v>
       </c>
       <c r="E96" s="3">
         <f t="shared" si="5"/>
-        <v>0.17929715515180492</v>
+        <v>0.17937971500419111</v>
       </c>
       <c r="F96">
         <f t="shared" si="7"/>
-        <v>0.21505422868351218</v>
+        <v>0.21528439783921194</v>
       </c>
       <c r="G96">
         <v>3854</v>
@@ -3097,11 +3097,11 @@
         <v>24</v>
       </c>
       <c r="J96">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K96">
         <f t="shared" si="4"/>
-        <v>177.33333333333334</v>
+        <v>178.33333333333334</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -3112,19 +3112,19 @@
         <v>845</v>
       </c>
       <c r="C97">
-        <v>4904</v>
+        <v>4900</v>
       </c>
       <c r="D97">
         <f t="shared" si="6"/>
-        <v>250846</v>
+        <v>250598</v>
       </c>
       <c r="E97" s="3">
         <f t="shared" si="5"/>
-        <v>0.17230831973898858</v>
+        <v>0.17244897959183675</v>
       </c>
       <c r="F97">
         <f t="shared" si="7"/>
-        <v>0.21066241434297289</v>
+        <v>0.21089962162084394</v>
       </c>
       <c r="G97">
         <v>3892</v>
@@ -3137,11 +3137,11 @@
         <v>25</v>
       </c>
       <c r="J97">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K97">
         <f t="shared" si="4"/>
-        <v>165.33333333333334</v>
+        <v>165.66666666666666</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -3149,22 +3149,22 @@
         <v>43948</v>
       </c>
       <c r="B98">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="C98">
-        <v>11093</v>
+        <v>11078</v>
       </c>
       <c r="D98">
         <f t="shared" si="6"/>
-        <v>261939</v>
+        <v>261676</v>
       </c>
       <c r="E98" s="3">
         <f t="shared" si="5"/>
-        <v>0.19192283421977824</v>
+        <v>0.19209243545766383</v>
       </c>
       <c r="F98">
         <f t="shared" si="7"/>
-        <v>0.2019834331737797</v>
+        <v>0.20216414804609578</v>
       </c>
       <c r="G98">
         <v>3875</v>
@@ -3192,19 +3192,19 @@
         <v>2107</v>
       </c>
       <c r="C99">
-        <v>12394</v>
+        <v>12375</v>
       </c>
       <c r="D99">
         <f t="shared" si="6"/>
-        <v>274333</v>
+        <v>274051</v>
       </c>
       <c r="E99" s="3">
         <f t="shared" si="5"/>
-        <v>0.17000161368404065</v>
+        <v>0.17026262626262625</v>
       </c>
       <c r="F99">
         <f t="shared" si="7"/>
-        <v>0.19281837965896256</v>
+        <v>0.1930340023449893</v>
       </c>
       <c r="G99">
         <v>3856</v>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="K99">
         <f t="shared" si="4"/>
-        <v>151.66666666666666</v>
+        <v>151.33333333333334</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -3229,22 +3229,22 @@
         <v>43950</v>
       </c>
       <c r="B100">
-        <v>2181</v>
+        <v>2185</v>
       </c>
       <c r="C100">
-        <v>12701</v>
+        <v>12694</v>
       </c>
       <c r="D100">
         <f t="shared" si="6"/>
-        <v>287034</v>
+        <v>286745</v>
       </c>
       <c r="E100" s="3">
         <f t="shared" si="5"/>
-        <v>0.17171876230218094</v>
+        <v>0.17212856467622498</v>
       </c>
       <c r="F100">
         <f t="shared" si="7"/>
-        <v>0.18536679430318723</v>
+        <v>0.18563212842543683</v>
       </c>
       <c r="G100">
         <v>3803</v>
@@ -3257,11 +3257,11 @@
         <v>25</v>
       </c>
       <c r="J100">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K100">
         <f t="shared" si="4"/>
-        <v>154.66666666666666</v>
+        <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -3269,22 +3269,22 @@
         <v>43951</v>
       </c>
       <c r="B101">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="C101">
-        <v>13784</v>
+        <v>13752</v>
       </c>
       <c r="D101">
         <f t="shared" si="6"/>
-        <v>300818</v>
+        <v>300497</v>
       </c>
       <c r="E101" s="3">
         <f t="shared" si="5"/>
-        <v>0.14901334881021475</v>
+        <v>0.14921465968586387</v>
       </c>
       <c r="F101">
         <f t="shared" si="7"/>
-        <v>0.1732336596983329</v>
+        <v>0.17347060460309258</v>
       </c>
       <c r="G101">
         <v>3716</v>
@@ -3297,11 +3297,11 @@
         <v>24</v>
       </c>
       <c r="J101">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K101">
         <f t="shared" si="4"/>
-        <v>148.33333333333334</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -3309,22 +3309,22 @@
         <v>43952</v>
       </c>
       <c r="B102">
-        <v>2086</v>
+        <v>2090</v>
       </c>
       <c r="C102">
-        <v>14322</v>
+        <v>14314</v>
       </c>
       <c r="D102">
         <f t="shared" si="6"/>
-        <v>315140</v>
+        <v>314811</v>
       </c>
       <c r="E102" s="3">
         <f t="shared" si="5"/>
-        <v>0.14565004887585534</v>
+        <v>0.14601089842112616</v>
       </c>
       <c r="F102">
         <f t="shared" si="7"/>
-        <v>0.16634005466453508</v>
+        <v>0.16659351440669215</v>
       </c>
       <c r="G102">
         <v>3601</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="K102">
         <f t="shared" si="4"/>
-        <v>159.33333333333334</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -3349,22 +3349,22 @@
         <v>43953</v>
       </c>
       <c r="B103">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C103">
-        <v>7444</v>
+        <v>7431</v>
       </c>
       <c r="D103">
         <f t="shared" si="6"/>
-        <v>322584</v>
+        <v>322242</v>
       </c>
       <c r="E103" s="3">
         <f t="shared" si="5"/>
-        <v>0.13997850617947341</v>
+        <v>0.13995424572735837</v>
       </c>
       <c r="F103">
         <f t="shared" si="7"/>
-        <v>0.16236528274314344</v>
+        <v>0.16261235367892976</v>
       </c>
       <c r="G103">
         <v>3617</v>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="K103">
         <f t="shared" si="4"/>
-        <v>151.66666666666666</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -3389,22 +3389,22 @@
         <v>43954</v>
       </c>
       <c r="B104">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C104">
-        <v>5097</v>
+        <v>5104</v>
       </c>
       <c r="D104">
         <f t="shared" si="6"/>
-        <v>327681</v>
+        <v>327346</v>
       </c>
       <c r="E104" s="3">
         <f t="shared" si="5"/>
-        <v>0.14361389052383755</v>
+        <v>0.14322100313479624</v>
       </c>
       <c r="F104">
         <f t="shared" si="7"/>
-        <v>0.16048675733715104</v>
+        <v>0.16069474123104185</v>
       </c>
       <c r="G104">
         <v>3539</v>
@@ -3429,22 +3429,22 @@
         <v>43955</v>
       </c>
       <c r="B105">
-        <v>1881</v>
+        <v>1890</v>
       </c>
       <c r="C105">
-        <v>12279</v>
+        <v>12293</v>
       </c>
       <c r="D105">
         <f t="shared" si="6"/>
-        <v>339960</v>
+        <v>339639</v>
       </c>
       <c r="E105" s="3">
         <f t="shared" si="5"/>
-        <v>0.15318837038846811</v>
+        <v>0.15374603432847964</v>
       </c>
       <c r="F105">
         <f t="shared" si="7"/>
-        <v>0.15486856102844107</v>
+        <v>0.15513769352128573</v>
       </c>
       <c r="G105">
         <v>3542</v>
@@ -3469,22 +3469,22 @@
         <v>43956</v>
       </c>
       <c r="B106">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="C106">
-        <v>12812</v>
+        <v>12840</v>
       </c>
       <c r="D106">
         <f t="shared" si="6"/>
-        <v>352772</v>
+        <v>352479</v>
       </c>
       <c r="E106" s="3">
         <f t="shared" si="5"/>
-        <v>0.13651264439587887</v>
+        <v>0.13598130841121495</v>
       </c>
       <c r="F106">
         <f t="shared" si="7"/>
-        <v>0.14947921314652149</v>
+        <v>0.149614933442138</v>
       </c>
       <c r="G106">
         <v>3562</v>
@@ -3509,22 +3509,22 @@
         <v>43957</v>
       </c>
       <c r="B107">
-        <v>1725</v>
+        <v>1716</v>
       </c>
       <c r="C107">
-        <v>13497</v>
+        <v>13450</v>
       </c>
       <c r="D107">
         <f t="shared" si="6"/>
-        <v>366269</v>
+        <v>365929</v>
       </c>
       <c r="E107" s="3">
         <f t="shared" si="5"/>
-        <v>0.12780617915092243</v>
+        <v>0.12758364312267659</v>
       </c>
       <c r="F107">
         <f t="shared" si="7"/>
-        <v>0.14222250268189562</v>
+        <v>0.14226358860375835</v>
       </c>
       <c r="G107">
         <v>3436</v>
@@ -3537,11 +3537,11 @@
         <v>21</v>
       </c>
       <c r="J107">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K107">
         <f t="shared" si="4"/>
-        <v>134.66666666666666</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -3549,22 +3549,22 @@
         <v>43958</v>
       </c>
       <c r="B108">
-        <v>1687</v>
+        <v>1689</v>
       </c>
       <c r="C108">
-        <v>13464</v>
+        <v>13439</v>
       </c>
       <c r="D108">
         <f t="shared" si="6"/>
-        <v>379733</v>
+        <v>379368</v>
       </c>
       <c r="E108" s="3">
         <f t="shared" si="5"/>
-        <v>0.12529708853238264</v>
+        <v>0.12567899397276583</v>
       </c>
       <c r="F108">
         <f t="shared" si="7"/>
-        <v>0.13814864094278653</v>
+        <v>0.1382257103371328</v>
       </c>
       <c r="G108">
         <v>3349</v>
@@ -3577,11 +3577,11 @@
         <v>19</v>
       </c>
       <c r="J108">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K108">
         <f t="shared" si="4"/>
-        <v>133.66666666666666</v>
+        <v>134.33333333333334</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -3589,22 +3589,22 @@
         <v>43959</v>
       </c>
       <c r="B109">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="C109">
-        <v>13539</v>
+        <v>13535</v>
       </c>
       <c r="D109">
         <f t="shared" si="6"/>
-        <v>393272</v>
+        <v>392903</v>
       </c>
       <c r="E109" s="3">
         <f t="shared" si="5"/>
-        <v>0.10872294851909299</v>
+        <v>0.10853343184336904</v>
       </c>
       <c r="F109">
         <f t="shared" si="7"/>
-        <v>0.13167460195566477</v>
+        <v>0.1316524099779747</v>
       </c>
       <c r="G109">
         <v>3229</v>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="K109">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>125.66666666666667</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -3629,22 +3629,22 @@
         <v>43960</v>
       </c>
       <c r="B110">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="C110">
-        <v>5917</v>
+        <v>5901</v>
       </c>
       <c r="D110">
         <f t="shared" si="6"/>
-        <v>399189</v>
+        <v>398804</v>
       </c>
       <c r="E110" s="3">
         <f t="shared" si="5"/>
-        <v>0.1167821531181342</v>
+        <v>0.11608201999661075</v>
       </c>
       <c r="F110">
         <f t="shared" si="7"/>
-        <v>0.12971738137197311</v>
+        <v>0.12964656095713278</v>
       </c>
       <c r="G110">
         <v>3128</v>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="K110">
         <f t="shared" si="4"/>
-        <v>114.33333333333333</v>
+        <v>114.66666666666667</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -3669,22 +3669,22 @@
         <v>43961</v>
       </c>
       <c r="B111">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C111">
-        <v>3201</v>
+        <v>3190</v>
       </c>
       <c r="D111">
         <f t="shared" si="6"/>
-        <v>402390</v>
+        <v>401994</v>
       </c>
       <c r="E111" s="3">
         <f t="shared" si="5"/>
-        <v>0.12152452358637926</v>
+        <v>0.12100313479623824</v>
       </c>
       <c r="F111">
         <f t="shared" si="7"/>
-        <v>0.12841826285989641</v>
+        <v>0.12834905154860143</v>
       </c>
       <c r="G111">
         <v>3102</v>
@@ -3709,22 +3709,22 @@
         <v>43962</v>
       </c>
       <c r="B112">
-        <v>1317</v>
+        <v>1310</v>
       </c>
       <c r="C112">
-        <v>12014</v>
+        <v>11988</v>
       </c>
       <c r="D112">
         <f t="shared" si="6"/>
-        <v>414404</v>
+        <v>413982</v>
       </c>
       <c r="E112" s="3">
         <f t="shared" si="5"/>
-        <v>0.10962210754120193</v>
+        <v>0.10927594260927594</v>
       </c>
       <c r="F112">
         <f t="shared" si="7"/>
-        <v>0.12129923163720381</v>
+        <v>0.12107394105699258</v>
       </c>
       <c r="G112">
         <v>3127</v>
@@ -3737,11 +3737,11 @@
         <v>20</v>
       </c>
       <c r="J112">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K112">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -3749,22 +3749,22 @@
         <v>43963</v>
       </c>
       <c r="B113">
-        <v>1468</v>
+        <v>1472</v>
       </c>
       <c r="C113">
-        <v>13359</v>
+        <v>13377</v>
       </c>
       <c r="D113">
         <f t="shared" si="6"/>
-        <v>427763</v>
+        <v>427359</v>
       </c>
       <c r="E113" s="3">
         <f t="shared" si="5"/>
-        <v>0.10988846470544203</v>
+        <v>0.11003962024370188</v>
       </c>
       <c r="F113">
         <f t="shared" si="7"/>
-        <v>0.11666733341334294</v>
+        <v>0.11654647435897436</v>
       </c>
       <c r="G113">
         <v>3101</v>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="K113">
         <f t="shared" si="4"/>
-        <v>118.33333333333333</v>
+        <v>119.33333333333333</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
@@ -3789,22 +3789,22 @@
         <v>43964</v>
       </c>
       <c r="B114">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="C114">
-        <v>13922</v>
+        <v>13891</v>
       </c>
       <c r="D114">
         <f t="shared" si="6"/>
-        <v>441685</v>
+        <v>441250</v>
       </c>
       <c r="E114" s="3">
         <f t="shared" si="5"/>
-        <v>9.4957621031460993E-2</v>
+        <v>9.4881578000143976E-2</v>
       </c>
       <c r="F114">
         <f t="shared" si="7"/>
-        <v>0.11066617163466638</v>
+        <v>0.11058005071626771</v>
       </c>
       <c r="G114">
         <v>2859</v>
@@ -3817,11 +3817,11 @@
         <v>18</v>
       </c>
       <c r="J114">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K114">
         <f t="shared" si="4"/>
-        <v>114.33333333333333</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -3829,22 +3829,22 @@
         <v>43965</v>
       </c>
       <c r="B115">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="C115">
-        <v>13161</v>
+        <v>13218</v>
       </c>
       <c r="D115">
         <f t="shared" si="6"/>
-        <v>454846</v>
+        <v>454468</v>
       </c>
       <c r="E115" s="3">
         <f t="shared" si="5"/>
-        <v>9.8472760428538864E-2</v>
+        <v>9.7896807383870479E-2</v>
       </c>
       <c r="F115">
         <f t="shared" si="7"/>
-        <v>0.10590709996937947</v>
+        <v>0.10564580559254327</v>
       </c>
       <c r="G115">
         <v>2767</v>
@@ -3857,11 +3857,11 @@
         <v>18</v>
       </c>
       <c r="J115">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K115">
         <f t="shared" ref="K115:K120" si="9">AVERAGE(J113:J115)</f>
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -3869,22 +3869,22 @@
         <v>43966</v>
       </c>
       <c r="B116">
-        <v>1130</v>
+        <v>1125</v>
       </c>
       <c r="C116">
-        <v>13763</v>
+        <v>13722</v>
       </c>
       <c r="D116">
         <f t="shared" si="6"/>
-        <v>468609</v>
+        <v>468190</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="5"/>
-        <v>8.2104192399912804E-2</v>
+        <v>8.19851333624836E-2</v>
       </c>
       <c r="F116">
         <f t="shared" si="7"/>
-        <v>0.10105260363433638</v>
+        <v>0.10081421759400694</v>
       </c>
       <c r="G116">
         <v>2692</v>
@@ -3897,11 +3897,11 @@
         <v>17</v>
       </c>
       <c r="J116" s="2">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K116">
         <f t="shared" si="9"/>
-        <v>105.33333333333333</v>
+        <v>107.33333333333333</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -3909,22 +3909,22 @@
         <v>43967</v>
       </c>
       <c r="B117">
-        <v>661</v>
+        <v>672</v>
       </c>
       <c r="C117">
-        <v>7008</v>
+        <v>7154</v>
       </c>
       <c r="D117">
         <f t="shared" si="6"/>
-        <v>475617</v>
+        <v>475344</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="5"/>
-        <v>9.4320776255707769E-2</v>
+        <v>9.393346379647749E-2</v>
       </c>
       <c r="F117">
         <f t="shared" si="7"/>
-        <v>9.9217564243470974E-2</v>
+        <v>9.8993990070551346E-2</v>
       </c>
       <c r="G117">
         <v>2597</v>
@@ -3937,11 +3937,11 @@
         <v>18</v>
       </c>
       <c r="J117" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K117">
         <f t="shared" si="9"/>
-        <v>97.333333333333329</v>
+        <v>99</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -3949,22 +3949,22 @@
         <v>43968</v>
       </c>
       <c r="B118" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C118" s="2">
-        <v>4283</v>
+        <v>4279</v>
       </c>
       <c r="D118">
         <f t="shared" ref="D118:D123" si="11">C118+D117</f>
-        <v>479900</v>
+        <v>479623</v>
       </c>
       <c r="E118" s="3">
         <f t="shared" si="5"/>
-        <v>8.8956339014709312E-2</v>
+        <v>8.8572096284178545E-2</v>
       </c>
       <c r="F118" s="2">
         <f t="shared" si="7"/>
-        <v>9.7729325248355051E-2</v>
+        <v>9.7515103891586907E-2</v>
       </c>
       <c r="G118" s="2">
         <v>2533</v>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="K118">
         <f t="shared" si="9"/>
-        <v>92.333333333333329</v>
+        <v>93.666666666666671</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -3989,22 +3989,22 @@
         <v>43969</v>
       </c>
       <c r="B119" s="2">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="C119" s="2">
-        <v>13369</v>
+        <v>13420</v>
       </c>
       <c r="D119">
         <f t="shared" si="11"/>
-        <v>493269</v>
+        <v>493043</v>
       </c>
       <c r="E119" s="3">
         <f t="shared" ref="E119" si="12">B119/C119</f>
-        <v>9.918468097838283E-2</v>
+        <v>9.8584202682563335E-2</v>
       </c>
       <c r="F119" s="2">
         <f t="shared" ref="F119" si="13">IFERROR(SUMPRODUCT(C113:C119,E113:E119)/SUM(C113:C119),"")</f>
-        <v>9.6164331452482085E-2</v>
+        <v>9.591328214922655E-2</v>
       </c>
       <c r="G119" s="2">
         <v>2472</v>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="K119">
         <f t="shared" si="9"/>
-        <v>84.666666666666671</v>
+        <v>85</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -4029,22 +4029,22 @@
         <v>43970</v>
       </c>
       <c r="B120" s="2">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C120" s="2">
-        <v>12253</v>
+        <v>12304</v>
       </c>
       <c r="D120">
         <f t="shared" si="11"/>
-        <v>505522</v>
+        <v>505347</v>
       </c>
       <c r="E120" s="3">
         <f t="shared" ref="E120" si="14">B120/C120</f>
-        <v>8.9365869582959279E-2</v>
+        <v>8.8832899869960985E-2</v>
       </c>
       <c r="F120" s="2">
         <f t="shared" ref="F120:F125" si="15">IFERROR(SUMPRODUCT(C114:C120,E114:E120)/SUM(C114:C120),"")</f>
-        <v>9.2735246080839523E-2</v>
+        <v>9.2373185618300255E-2</v>
       </c>
       <c r="G120" s="2">
         <v>2518</v>
@@ -4057,11 +4057,11 @@
         <v>13</v>
       </c>
       <c r="J120" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K120">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>78.666666666666671</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -4072,19 +4072,19 @@
         <v>1013</v>
       </c>
       <c r="C121" s="2">
-        <v>12248</v>
+        <v>12459</v>
       </c>
       <c r="D121">
         <f t="shared" si="11"/>
-        <v>517770</v>
+        <v>517806</v>
       </c>
       <c r="E121" s="3">
-        <f>B121/C121</f>
-        <v>8.2707380796864793E-2</v>
+        <f t="shared" ref="E121:E126" si="16">B121/C121</f>
+        <v>8.1306685929849909E-2</v>
       </c>
       <c r="F121" s="2">
         <f t="shared" si="15"/>
-        <v>9.0714332654268259E-2</v>
+        <v>9.0117038507759026E-2</v>
       </c>
       <c r="G121" s="2">
         <v>2396</v>
@@ -4097,11 +4097,11 @@
         <v>15</v>
       </c>
       <c r="J121" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K121">
-        <f>AVERAGE(J119:J121)</f>
-        <v>78.333333333333329</v>
+        <f t="shared" ref="K121:K127" si="17">AVERAGE(J119:J121)</f>
+        <v>79.333333333333329</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -4109,22 +4109,22 @@
         <v>43972</v>
       </c>
       <c r="B122" s="2">
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="C122" s="2">
-        <v>10630</v>
+        <v>11455</v>
       </c>
       <c r="D122">
         <f t="shared" si="11"/>
-        <v>528400</v>
+        <v>529261</v>
       </c>
       <c r="E122" s="3">
-        <f>B122/C122</f>
-        <v>9.0216368767638763E-2</v>
+        <f t="shared" si="16"/>
+        <v>8.450458315146224E-2</v>
       </c>
       <c r="F122" s="2">
         <f t="shared" si="15"/>
-        <v>8.9254153411099324E-2</v>
+        <v>8.7882555854157468E-2</v>
       </c>
       <c r="G122" s="2">
         <v>2323</v>
@@ -4137,10 +4137,10 @@
         <v>13</v>
       </c>
       <c r="J122" s="2">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K122">
-        <f>AVERAGE(J120:J122)</f>
+        <f t="shared" si="17"/>
         <v>70.666666666666671</v>
       </c>
     </row>
@@ -4149,39 +4149,39 @@
         <v>43973</v>
       </c>
       <c r="B123" s="2">
-        <v>806</v>
+        <v>869</v>
       </c>
       <c r="C123" s="2">
-        <v>8920</v>
+        <v>10698</v>
       </c>
       <c r="D123">
         <f t="shared" si="11"/>
-        <v>537320</v>
+        <v>539959</v>
       </c>
       <c r="E123" s="3">
-        <f>B123/C123</f>
-        <v>9.0358744394618828E-2</v>
+        <f t="shared" si="16"/>
+        <v>8.1230136474107303E-2</v>
       </c>
       <c r="F123" s="2">
         <f t="shared" si="15"/>
-        <v>9.0829707033808271E-2</v>
+        <v>8.8018503810837548E-2</v>
       </c>
       <c r="G123" s="2">
         <v>2237</v>
       </c>
       <c r="H123">
-        <f>AVERAGE(G121:G123)</f>
+        <f t="shared" ref="H123:H129" si="18">AVERAGE(G121:G123)</f>
         <v>2318.6666666666665</v>
       </c>
       <c r="I123" s="2">
         <v>12</v>
       </c>
       <c r="J123" s="2">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="K123">
-        <f>AVERAGE(J121:J123)</f>
-        <v>68.333333333333329</v>
+        <f t="shared" si="17"/>
+        <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -4189,39 +4189,39 @@
         <v>43974</v>
       </c>
       <c r="B124" s="2">
-        <v>349</v>
+        <v>400</v>
       </c>
       <c r="C124" s="2">
-        <v>4031</v>
+        <v>4908</v>
       </c>
       <c r="D124">
         <f>C124+D123</f>
-        <v>541351</v>
+        <v>544867</v>
       </c>
       <c r="E124" s="3">
-        <f>B124/C124</f>
-        <v>8.657901265194741E-2</v>
+        <f t="shared" si="16"/>
+        <v>8.1499592502037491E-2</v>
       </c>
       <c r="F124" s="2">
         <f t="shared" si="15"/>
-        <v>9.0196853987282083E-2</v>
+        <v>8.6949642564331228E-2</v>
       </c>
       <c r="G124" s="2">
         <v>2169</v>
       </c>
       <c r="H124">
-        <f>AVERAGE(G122:G124)</f>
+        <f t="shared" si="18"/>
         <v>2243</v>
       </c>
       <c r="I124" s="2">
         <v>9</v>
       </c>
       <c r="J124" s="2">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="K124">
-        <f>AVERAGE(J122:J124)</f>
-        <v>57</v>
+        <f t="shared" si="17"/>
+        <v>67.666666666666671</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
@@ -4229,32 +4229,39 @@
         <v>43975</v>
       </c>
       <c r="B125" s="2">
-        <v>190</v>
+        <v>283</v>
       </c>
       <c r="C125" s="2">
-        <v>3042</v>
+        <v>4106</v>
       </c>
       <c r="D125">
         <f>C125+D124</f>
-        <v>544393</v>
+        <v>548973</v>
       </c>
       <c r="E125" s="3">
-        <f>B125/C125</f>
-        <v>6.2458908612754764E-2</v>
+        <f t="shared" si="16"/>
+        <v>6.8923526546517289E-2</v>
       </c>
       <c r="F125" s="2">
         <f t="shared" si="15"/>
-        <v>8.8970896066239744E-2</v>
+        <v>8.5782263878875276E-2</v>
       </c>
       <c r="G125" s="2">
         <v>2132</v>
       </c>
       <c r="H125">
-        <f>AVERAGE(G123:G125)</f>
+        <f t="shared" si="18"/>
         <v>2179.3333333333335</v>
       </c>
       <c r="I125" s="2">
         <v>8</v>
+      </c>
+      <c r="J125" s="2">
+        <v>55</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="17"/>
+        <v>65</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -4262,32 +4269,145 @@
         <v>43976</v>
       </c>
       <c r="B126" s="2">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="C126" s="2">
-        <v>1065</v>
+        <v>3110</v>
       </c>
       <c r="D126">
         <f>C126+D125</f>
-        <v>545458</v>
+        <v>552083</v>
       </c>
       <c r="E126" s="3">
-        <f>B126/C126</f>
-        <v>6.3849765258215965E-2</v>
+        <f t="shared" si="16"/>
+        <v>6.591639871382636E-2</v>
       </c>
       <c r="F126" s="2">
-        <f t="shared" ref="F126" si="16">IFERROR(SUMPRODUCT(C120:C126,E120:E126)/SUM(C120:C126),"")</f>
-        <v>8.5841844066757364E-2</v>
+        <f t="shared" ref="F126" si="19">IFERROR(SUMPRODUCT(C120:C126,E120:E126)/SUM(C120:C126),"")</f>
+        <v>8.182588075880759E-2</v>
       </c>
       <c r="G126" s="2">
         <v>2108</v>
       </c>
       <c r="H126">
-        <f>AVERAGE(G124:G126)</f>
+        <f t="shared" si="18"/>
         <v>2136.3333333333335</v>
       </c>
       <c r="I126" s="2">
         <v>8</v>
+      </c>
+      <c r="J126" s="2">
+        <v>52</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="17"/>
+        <v>56.333333333333336</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B127">
+        <v>847</v>
+      </c>
+      <c r="C127">
+        <v>10122</v>
+      </c>
+      <c r="D127">
+        <f>C127+D126</f>
+        <v>562205</v>
+      </c>
+      <c r="E127" s="3">
+        <f t="shared" ref="E127" si="20">B127/C127</f>
+        <v>8.3679114799446744E-2</v>
+      </c>
+      <c r="F127" s="2">
+        <f t="shared" ref="F127" si="21">IFERROR(SUMPRODUCT(C121:C127,E121:E127)/SUM(C121:C127),"")</f>
+        <v>8.063948784691688E-2</v>
+      </c>
+      <c r="G127">
+        <v>2106</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="18"/>
+        <v>2115.3333333333335</v>
+      </c>
+      <c r="I127">
+        <v>8</v>
+      </c>
+      <c r="J127" s="2">
+        <v>61</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="17"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B128" s="2">
+        <v>494</v>
+      </c>
+      <c r="C128" s="2">
+        <v>6945</v>
+      </c>
+      <c r="D128">
+        <f>C128+D127</f>
+        <v>569150</v>
+      </c>
+      <c r="E128" s="3">
+        <f t="shared" ref="E128" si="22">B128/C128</f>
+        <v>7.1130309575233988E-2</v>
+      </c>
+      <c r="F128" s="2">
+        <f t="shared" ref="F128" si="23">IFERROR(SUMPRODUCT(C122:C128,E122:E128)/SUM(C122:C128),"")</f>
+        <v>7.9191336865067005E-2</v>
+      </c>
+      <c r="G128" s="2">
+        <v>2112</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="18"/>
+        <v>2108.6666666666665</v>
+      </c>
+      <c r="I128" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B129" s="2">
+        <v>156</v>
+      </c>
+      <c r="C129" s="2">
+        <v>2580</v>
+      </c>
+      <c r="D129">
+        <f>C129+D128</f>
+        <v>571730</v>
+      </c>
+      <c r="E129" s="3">
+        <f t="shared" ref="E129" si="24">B129/C129</f>
+        <v>6.0465116279069767E-2</v>
+      </c>
+      <c r="F129" s="2">
+        <f t="shared" ref="F129" si="25">IFERROR(SUMPRODUCT(C123:C129,E123:E129)/SUM(C123:C129),"")</f>
+        <v>7.6620593844922175E-2</v>
+      </c>
+      <c r="G129" s="2">
+        <v>1991</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="18"/>
+        <v>2069.6666666666665</v>
+      </c>
+      <c r="I129" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>